<commit_message>
new feature: excel download
</commit_message>
<xml_diff>
--- a/src/asset/demo.xlsx
+++ b/src/asset/demo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29064f94e858990c/文件/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liya\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{ED9712FF-174A-4A45-80A7-24651AF4F6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7583F61C-E518-4CDC-BBDC-20405DE5F24A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE6BAB9-05C4-42C4-A87D-25C2C4E8A1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{57AB225E-2596-4CA5-AE5D-AF00F3349490}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="施工照片" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">施工照片!$A$1:$B$16</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">施工照片!$A$1:$B$22</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>施工照片</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -268,11 +268,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2774,15 +2774,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>571502</xdr:colOff>
+      <xdr:colOff>932330</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>44825</xdr:rowOff>
+      <xdr:rowOff>98614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3360189</xdr:colOff>
+      <xdr:colOff>3001601</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1042148</xdr:rowOff>
+      <xdr:rowOff>779930</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2805,8 +2805,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="571502" y="1905001"/>
-          <a:ext cx="2788687" cy="3664323"/>
+          <a:off x="932330" y="1972238"/>
+          <a:ext cx="2069271" cy="2554939"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2818,9 +2818,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2583659</xdr:colOff>
+      <xdr:colOff>2278859</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>464345</xdr:rowOff>
+      <xdr:rowOff>249192</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="838614" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -2836,7 +2836,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2583659" y="5024439"/>
+          <a:off x="2278859" y="4220557"/>
           <a:ext cx="838614" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2883,15 +2883,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>24618</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>357185</xdr:rowOff>
+      <xdr:colOff>618565</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>195820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3831478</xdr:colOff>
+      <xdr:colOff>3714937</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>546847</xdr:rowOff>
+      <xdr:rowOff>658320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2914,8 +2914,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24618" y="5995985"/>
-          <a:ext cx="3806860" cy="2861144"/>
+          <a:off x="618565" y="4749891"/>
+          <a:ext cx="3096372" cy="2327158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2927,9 +2927,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3071813</xdr:colOff>
+      <xdr:colOff>2883554</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>250028</xdr:rowOff>
+      <xdr:rowOff>294852</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="838614" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -2945,7 +2945,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3071813" y="8560591"/>
+          <a:off x="2883554" y="6713581"/>
           <a:ext cx="838614" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -7232,6 +7232,641 @@
               <a:srgbClr val="FFFF00"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2176096</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="124" name="文字方塊 123">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{015DE826-B4B7-4DDC-B34E-368EEF1126DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2176096" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2293327</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="125" name="文字方塊 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA40CAD-9EFD-434B-B3DB-2407143C4F4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6058055" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2176097</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="126" name="文字方塊 125">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{045BFE30-4E9A-4B48-A356-E460D92537D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2176097" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2293327</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="127" name="文字方塊 126">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6625FF7-6C3E-468B-8D25-D50E481BC202}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6058055" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2190750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="128" name="文字方塊 127">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6FC4314-C4BC-4262-865C-410E728B144E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190750" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2146789</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="129" name="文字方塊 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43DFF679-8AE1-451A-A925-B8006ED95FE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2146789" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2234711</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="134" name="文字方塊 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECFD1582-30FE-4B68-83F6-A6A58E5835F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2234711" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2249365</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="135" name="文字方塊 134">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BCE24D-F5FB-4B6A-A192-556246F165D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6059813" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2190750</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="140" name="文字方塊 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35F8C633-3B8A-4ED5-80EC-21E113A0E3DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2190750" y="4554071"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>618565</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>195820</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3096372" cy="2327158"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="141" name="圖片 140">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{746A91E1-4DE5-4F09-8150-09AC4FF58F75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="618565" y="4749891"/>
+          <a:ext cx="3096372" cy="2327158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2883554</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>294852</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="838614" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="146" name="文字方塊 145">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A10594A-6259-404D-B1CC-FA2B71557F69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2883554" y="6713581"/>
+          <a:ext cx="838614" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-TW" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>110.10.28</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7537,10 +8172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBC78528-4887-43D5-A5D7-29466703AEA2}">
-  <dimension ref="A2:B16"/>
+  <dimension ref="A2:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
@@ -7550,14 +8185,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
     </row>
     <row r="3" spans="1:2" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
     </row>
     <row r="4" spans="1:2" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -7585,58 +8220,83 @@
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+    <row r="10" spans="1:2" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+    <row r="11" spans="1:2" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8"/>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+    <row r="12" spans="1:2" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="8"/>
       <c r="B12" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="8"/>
       <c r="B13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="64.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+    <row r="14" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="107.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:2" ht="63.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
       <c r="B15" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="85.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:2" ht="63.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="17" spans="1:2" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="63.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="62.85" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A17:A20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>